<commit_message>
Scientific properties mapping spreadsheet updated to use specialization identifiers
</commit_message>
<xml_diff>
--- a/mappings/cmip5-ocean-scientific-properties.xlsx
+++ b/mappings/cmip5-ocean-scientific-properties.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="460" windowWidth="19840" windowHeight="17300"/>
+    <workbookView xWindow="1960" yWindow="460" windowWidth="19840" windowHeight="17300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -348,7 +348,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -378,12 +378,6 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
@@ -519,7 +513,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -548,9 +542,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1747,7 +1738,7 @@
   <dimension ref="A1:C70"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1885,7 +1876,7 @@
       <c r="B13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>56</v>
       </c>
     </row>

</xml_diff>